<commit_message>
ok to excel file
</commit_message>
<xml_diff>
--- a/send_list.xlsx
+++ b/send_list.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="540" windowWidth="27495" windowHeight="12210"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="80">
   <si>
     <t>ok</t>
   </si>
@@ -259,38 +259,39 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color theme="10"/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -312,23 +313,23 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Обычный" xfId="0"/>
+    <cellStyle builtinId="8" name="Гиперссылка" xfId="1"/>
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -337,7 +338,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -348,34 +349,34 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -384,17 +385,12 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица2" displayName="Таблица2" ref="A1:AU5" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Таблица2" headerRowCount="1" id="1" name="Таблица2" ref="A1:AU5" totalsRowShown="0">
   <autoFilter ref="A1:AU5"/>
   <tableColumns count="47">
     <tableColumn id="1" name="ok"/>
@@ -405,7 +401,7 @@
     <tableColumn id="6" name="Ауд"/>
     <tableColumn id="7" name="Школа"/>
     <tableColumn id="8" name="Год р."/>
-    <tableColumn id="9" name="email" dataCellStyle="Гиперссылка"/>
+    <tableColumn dataCellStyle="Гиперссылка" id="9" name="email"/>
     <tableColumn id="10" name="пол"/>
     <tableColumn id="11" name="а"/>
     <tableColumn id="12" name="subject">
@@ -429,22 +425,22 @@
     <tableColumn id="24" name="mx7"/>
     <tableColumn id="25" name="mx8"/>
     <tableColumn id="26" name="mx9"/>
-    <tableColumn id="27" name="mxtot" dataDxfId="12">
+    <tableColumn dataDxfId="12" id="27" name="mxtot">
       <calculatedColumnFormula>SUM(R2:Z2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" name="pl1" dataDxfId="11"/>
-    <tableColumn id="29" name="pl2" dataDxfId="10"/>
-    <tableColumn id="30" name="pl3" dataDxfId="9"/>
-    <tableColumn id="31" name="pl4" dataDxfId="8"/>
-    <tableColumn id="32" name="pl5" dataDxfId="7"/>
-    <tableColumn id="33" name="pl6" dataDxfId="6"/>
-    <tableColumn id="34" name="pl7" dataDxfId="5"/>
-    <tableColumn id="35" name="pl8" dataDxfId="4"/>
-    <tableColumn id="36" name="pl9" dataDxfId="3"/>
-    <tableColumn id="37" name="pltot" dataDxfId="2">
+    <tableColumn dataDxfId="11" id="28" name="pl1"/>
+    <tableColumn dataDxfId="10" id="29" name="pl2"/>
+    <tableColumn dataDxfId="9" id="30" name="pl3"/>
+    <tableColumn dataDxfId="8" id="31" name="pl4"/>
+    <tableColumn dataDxfId="7" id="32" name="pl5"/>
+    <tableColumn dataDxfId="6" id="33" name="pl6"/>
+    <tableColumn dataDxfId="5" id="34" name="pl7"/>
+    <tableColumn dataDxfId="4" id="35" name="pl8"/>
+    <tableColumn dataDxfId="3" id="36" name="pl9"/>
+    <tableColumn dataDxfId="2" id="37" name="pltot">
       <calculatedColumnFormula>ROUND(IF(AB2="+",1,IF(AB2="+.",1,IF(AB2="+-",0.8,IF(AB2="+/2",0.5,IF(AB2="-+",0.1,IF(AB2="-.",0,IF(AB2="-",0,IF(AB2="0",0,IF(AB2="",0,"?")))))))))+IF(AC2="+",1,IF(AC2="+.",1,IF(AC2="+-",0.8,IF(AC2="+/2",0.5,IF(AC2="-+",0.1,IF(AC2="-.",0,IF(AC2="-",0,IF(AC2="0",0,IF(AC2="",0,"?")))))))))+IF(AD2="+",1,IF(AD2="+.",1,IF(AD2="+-",0.8,IF(AD2="+/2",0.5,IF(AD2="-+",0.1,IF(AD2="-.",0,IF(AD2="-",0,IF(AD2="0",0,IF(AD2="",0,"?")))))))))+IF(AE2="+",1,IF(AE2="+.",1,IF(AE2="+-",0.8,IF(AE2="+/2",0.5,IF(AE2="-+",0.1,IF(AE2="-.",0,IF(AE2="-",0,IF(AE2="0",0,IF(AE2="",0,"?")))))))))+IF(AF2="+",1,IF(AF2="+.",1,IF(AF2="+-",0.8,IF(AF2="+/2",0.5,IF(AF2="-+",0.1,IF(AF2="-.",0,IF(AF2="-",0,IF(AF2="0",0,IF(AF2="",0,"?")))))))))+IF(AG2="+",1,IF(AG2="+.",1,IF(AG2="+-",0.8,IF(AG2="+/2",0.5,IF(AG2="-+",0.1,IF(AG2="-.",0,IF(AG2="-",0,IF(AG2="0",0,IF(AG2="",0,"?")))))))))+IF(AH2="+",1,IF(AH2="+.",1,IF(AH2="+-",0.8,IF(AH2="+/2",0.5,IF(AH2="-+",0.1,IF(AH2="-.",0,IF(AH2="-",0,IF(AH2="0",0,IF(AH2="",0,"?")))))))))+IF(AI2="+",1,IF(AI2="+.",1,IF(AI2="+-",0.8,IF(AI2="+/2",0.5,IF(AI2="-+",0.1,IF(AI2="-.",0,IF(AI2="-",0,IF(AI2="0",0,IF(AI2="",0,"?")))))))))+IF(AJ2="+",1,IF(AJ2="+.",1,IF(AJ2="+-",0.8,IF(AJ2="+/2",0.5,IF(AJ2="-+",0.1,IF(AJ2="-.",0,IF(AJ2="-",0,IF(AJ2="0",0,IF(AJ2="",0,"?"))))))))),2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" name="bl1" dataDxfId="1">
+    <tableColumn dataDxfId="1" id="38" name="bl1">
       <calculatedColumnFormula>ROUND(IF(AB2="+",1,IF(AB2="+.",1,IF(AB2="+-",0.8,IF(AB2="+/2",0.5,IF(AB2="-+",0.1,IF(AB2="-.",0,IF(AB2="-",0,IF(AB2="0",0,IF(AB2="",0,"?")))))))))*R2,2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="39" name="bl2">
@@ -471,11 +467,11 @@
     <tableColumn id="46" name="bl9">
       <calculatedColumnFormula>ROUND(IF(AJ2="+",1,IF(AJ2="+.",1,IF(AJ2="+-",0.8,IF(AJ2="+/2",0.5,IF(AJ2="-+",0.1,IF(AJ2="-.",0,IF(AJ2="-",0,IF(AJ2="0",0,IF(AJ2="",0,"?")))))))))*Z2,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="47" name="bltot" dataDxfId="0">
+    <tableColumn dataDxfId="0" id="47" name="bltot">
       <calculatedColumnFormula>SUM(AL2:AT2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
@@ -765,43 +761,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:AU5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" customWidth="1"/>
-    <col min="11" max="11" width="4.140625" customWidth="1"/>
-    <col min="12" max="12" width="54.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.140625" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" customWidth="1"/>
-    <col min="15" max="15" width="41" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.140625" customWidth="1"/>
-    <col min="18" max="26" width="6.85546875" customWidth="1"/>
-    <col min="27" max="27" width="8.42578125" style="3" customWidth="1"/>
-    <col min="28" max="36" width="5.85546875" style="1" customWidth="1"/>
-    <col min="37" max="37" width="7.42578125" style="3" customWidth="1"/>
-    <col min="38" max="38" width="5.85546875" customWidth="1"/>
-    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="40" max="46" width="5.85546875" customWidth="1"/>
-    <col min="47" max="47" width="7.42578125" style="3" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="5.28515625"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="5.5703125"/>
+    <col customWidth="1" max="3" min="3" width="18"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="13.5703125"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" width="10.42578125"/>
+    <col customWidth="1" max="6" min="6" width="6.5703125"/>
+    <col customWidth="1" max="7" min="7" width="9.28515625"/>
+    <col customWidth="1" max="8" min="8" width="8.42578125"/>
+    <col bestFit="1" customWidth="1" max="9" min="9" width="17"/>
+    <col customWidth="1" max="10" min="10" width="6.5703125"/>
+    <col customWidth="1" max="11" min="11" width="4.140625"/>
+    <col bestFit="1" customWidth="1" max="12" min="12" width="54.140625"/>
+    <col customWidth="1" max="13" min="13" width="4.140625"/>
+    <col customWidth="1" max="14" min="14" width="9.5703125"/>
+    <col bestFit="1" customWidth="1" max="15" min="15" width="41"/>
+    <col bestFit="1" customWidth="1" max="16" min="16" width="17.85546875"/>
+    <col customWidth="1" max="17" min="17" width="5.140625"/>
+    <col customWidth="1" max="26" min="18" width="6.85546875"/>
+    <col customWidth="1" max="27" min="27" style="3" width="8.42578125"/>
+    <col customWidth="1" max="36" min="28" style="1" width="5.85546875"/>
+    <col customWidth="1" max="37" min="37" style="3" width="7.42578125"/>
+    <col customWidth="1" max="38" min="38" width="5.85546875"/>
+    <col bestFit="1" customWidth="1" max="39" min="39" width="7.42578125"/>
+    <col customWidth="1" max="46" min="40" width="5.85546875"/>
+    <col customWidth="1" max="47" min="47" style="3" width="7.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -944,10 +944,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
+    <row r="2" spans="1:47">
       <c r="B2" t="s">
         <v>47</v>
       </c>
@@ -960,13 +957,13 @@
       <c r="E2" t="s">
         <v>50</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="n">
         <v>305</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="n">
         <v>123</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="n">
         <v>2001</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -975,13 +972,13 @@
       <c r="J2" t="s">
         <v>52</v>
       </c>
-      <c r="L2" t="str">
+      <c r="L2">
         <f>"Собеседования в 7-й математический класс 179-й школы"</f>
-        <v>Собеседования в 7-й математический класс 179-й школы</v>
-      </c>
-      <c r="M2" t="str">
+        <v/>
+      </c>
+      <c r="M2">
         <f>"|"</f>
-        <v>|</v>
+        <v/>
       </c>
       <c r="N2" t="s">
         <v>53</v>
@@ -992,40 +989,40 @@
       <c r="P2" t="s">
         <v>55</v>
       </c>
-      <c r="Q2" t="str">
+      <c r="Q2">
         <f>"|"</f>
-        <v>|</v>
-      </c>
-      <c r="R2">
-        <v>2</v>
-      </c>
-      <c r="S2">
-        <v>3</v>
-      </c>
-      <c r="T2">
-        <v>2</v>
-      </c>
-      <c r="U2">
-        <v>3</v>
-      </c>
-      <c r="V2">
-        <v>2</v>
-      </c>
-      <c r="W2">
-        <v>3</v>
-      </c>
-      <c r="X2">
-        <v>2</v>
-      </c>
-      <c r="Y2">
-        <v>3</v>
-      </c>
-      <c r="Z2">
+        <v/>
+      </c>
+      <c r="R2" t="n">
+        <v>2</v>
+      </c>
+      <c r="S2" t="n">
+        <v>3</v>
+      </c>
+      <c r="T2" t="n">
+        <v>2</v>
+      </c>
+      <c r="U2" t="n">
+        <v>3</v>
+      </c>
+      <c r="V2" t="n">
+        <v>2</v>
+      </c>
+      <c r="W2" t="n">
+        <v>3</v>
+      </c>
+      <c r="X2" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z2" t="n">
         <v>2</v>
       </c>
       <c r="AA2" s="3">
         <f>SUM(R2:Z2)</f>
-        <v>22</v>
+        <v/>
       </c>
       <c r="AB2" s="1" t="s">
         <v>56</v>
@@ -1050,50 +1047,53 @@
       </c>
       <c r="AK2" s="3">
         <f>ROUND(IF(AB2="+",1,IF(AB2="+.",1,IF(AB2="+-",0.8,IF(AB2="+/2",0.5,IF(AB2="-+",0.1,IF(AB2="-.",0,IF(AB2="-",0,IF(AB2="0",0,IF(AB2="",0,"?")))))))))+IF(AC2="+",1,IF(AC2="+.",1,IF(AC2="+-",0.8,IF(AC2="+/2",0.5,IF(AC2="-+",0.1,IF(AC2="-.",0,IF(AC2="-",0,IF(AC2="0",0,IF(AC2="",0,"?")))))))))+IF(AD2="+",1,IF(AD2="+.",1,IF(AD2="+-",0.8,IF(AD2="+/2",0.5,IF(AD2="-+",0.1,IF(AD2="-.",0,IF(AD2="-",0,IF(AD2="0",0,IF(AD2="",0,"?")))))))))+IF(AE2="+",1,IF(AE2="+.",1,IF(AE2="+-",0.8,IF(AE2="+/2",0.5,IF(AE2="-+",0.1,IF(AE2="-.",0,IF(AE2="-",0,IF(AE2="0",0,IF(AE2="",0,"?")))))))))+IF(AF2="+",1,IF(AF2="+.",1,IF(AF2="+-",0.8,IF(AF2="+/2",0.5,IF(AF2="-+",0.1,IF(AF2="-.",0,IF(AF2="-",0,IF(AF2="0",0,IF(AF2="",0,"?")))))))))+IF(AG2="+",1,IF(AG2="+.",1,IF(AG2="+-",0.8,IF(AG2="+/2",0.5,IF(AG2="-+",0.1,IF(AG2="-.",0,IF(AG2="-",0,IF(AG2="0",0,IF(AG2="",0,"?")))))))))+IF(AH2="+",1,IF(AH2="+.",1,IF(AH2="+-",0.8,IF(AH2="+/2",0.5,IF(AH2="-+",0.1,IF(AH2="-.",0,IF(AH2="-",0,IF(AH2="0",0,IF(AH2="",0,"?")))))))))+IF(AI2="+",1,IF(AI2="+.",1,IF(AI2="+-",0.8,IF(AI2="+/2",0.5,IF(AI2="-+",0.1,IF(AI2="-.",0,IF(AI2="-",0,IF(AI2="0",0,IF(AI2="",0,"?")))))))))+IF(AJ2="+",1,IF(AJ2="+.",1,IF(AJ2="+-",0.8,IF(AJ2="+/2",0.5,IF(AJ2="-+",0.1,IF(AJ2="-.",0,IF(AJ2="-",0,IF(AJ2="0",0,IF(AJ2="",0,"?"))))))))),2)</f>
-        <v>2.8</v>
+        <v/>
       </c>
       <c r="AL2">
-        <f t="shared" ref="AL2:AT5" si="0">ROUND(IF(AB2="+",1,IF(AB2="+.",1,IF(AB2="+-",0.8,IF(AB2="+/2",0.5,IF(AB2="-+",0.1,IF(AB2="-.",0,IF(AB2="-",0,IF(AB2="0",0,IF(AB2="",0,"?")))))))))*R2,2)</f>
-        <v>2</v>
+        <f>ROUND(IF(AB2="+",1,IF(AB2="+.",1,IF(AB2="+-",0.8,IF(AB2="+/2",0.5,IF(AB2="-+",0.1,IF(AB2="-.",0,IF(AB2="-",0,IF(AB2="0",0,IF(AB2="",0,"?")))))))))*R2,2)</f>
+        <v/>
       </c>
       <c r="AM2">
-        <f t="shared" si="0"/>
-        <v>2.4</v>
+        <f>ROUND(IF(AC2="+",1,IF(AC2="+.",1,IF(AC2="+-",0.8,IF(AC2="+/2",0.5,IF(AC2="-+",0.1,IF(AC2="-.",0,IF(AC2="-",0,IF(AC2="0",0,IF(AC2="",0,"?")))))))))*S2,2)</f>
+        <v/>
       </c>
       <c r="AN2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AD2="+",1,IF(AD2="+.",1,IF(AD2="+-",0.8,IF(AD2="+/2",0.5,IF(AD2="-+",0.1,IF(AD2="-.",0,IF(AD2="-",0,IF(AD2="0",0,IF(AD2="",0,"?")))))))))*T2,2)</f>
+        <v/>
       </c>
       <c r="AO2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AE2="+",1,IF(AE2="+.",1,IF(AE2="+-",0.8,IF(AE2="+/2",0.5,IF(AE2="-+",0.1,IF(AE2="-.",0,IF(AE2="-",0,IF(AE2="0",0,IF(AE2="",0,"?")))))))))*U2,2)</f>
+        <v/>
       </c>
       <c r="AP2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AF2="+",1,IF(AF2="+.",1,IF(AF2="+-",0.8,IF(AF2="+/2",0.5,IF(AF2="-+",0.1,IF(AF2="-.",0,IF(AF2="-",0,IF(AF2="0",0,IF(AF2="",0,"?")))))))))*V2,2)</f>
+        <v/>
       </c>
       <c r="AQ2">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>ROUND(IF(AG2="+",1,IF(AG2="+.",1,IF(AG2="+-",0.8,IF(AG2="+/2",0.5,IF(AG2="-+",0.1,IF(AG2="-.",0,IF(AG2="-",0,IF(AG2="0",0,IF(AG2="",0,"?")))))))))*W2,2)</f>
+        <v/>
       </c>
       <c r="AR2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AH2="+",1,IF(AH2="+.",1,IF(AH2="+-",0.8,IF(AH2="+/2",0.5,IF(AH2="-+",0.1,IF(AH2="-.",0,IF(AH2="-",0,IF(AH2="0",0,IF(AH2="",0,"?")))))))))*X2,2)</f>
+        <v/>
       </c>
       <c r="AS2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AI2="+",1,IF(AI2="+.",1,IF(AI2="+-",0.8,IF(AI2="+/2",0.5,IF(AI2="-+",0.1,IF(AI2="-.",0,IF(AI2="-",0,IF(AI2="0",0,IF(AI2="",0,"?")))))))))*Y2,2)</f>
+        <v/>
       </c>
       <c r="AT2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AJ2="+",1,IF(AJ2="+.",1,IF(AJ2="+-",0.8,IF(AJ2="+/2",0.5,IF(AJ2="-+",0.1,IF(AJ2="-.",0,IF(AJ2="-",0,IF(AJ2="0",0,IF(AJ2="",0,"?")))))))))*Z2,2)</f>
+        <v/>
       </c>
       <c r="AU2" s="3">
         <f>SUM(AL2:AT2)</f>
-        <v>7.4</v>
+        <v/>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
       <c r="B3" t="s">
         <v>60</v>
       </c>
@@ -1106,13 +1106,13 @@
       <c r="E3" t="s">
         <v>63</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="n">
         <v>306</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="n">
         <v>234</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="n">
         <v>2002</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -1121,13 +1121,13 @@
       <c r="J3" t="s">
         <v>52</v>
       </c>
-      <c r="L3" t="str">
+      <c r="L3">
         <f>"Собеседования в 7-й математический класс 179-й школы"</f>
-        <v>Собеседования в 7-й математический класс 179-й школы</v>
-      </c>
-      <c r="M3" t="str">
+        <v/>
+      </c>
+      <c r="M3">
         <f>"|"</f>
-        <v>|</v>
+        <v/>
       </c>
       <c r="N3" t="s">
         <v>53</v>
@@ -1138,40 +1138,40 @@
       <c r="P3" t="s">
         <v>55</v>
       </c>
-      <c r="Q3" t="str">
+      <c r="Q3">
         <f>"|"</f>
-        <v>|</v>
-      </c>
-      <c r="R3">
-        <v>2</v>
-      </c>
-      <c r="S3">
-        <v>3</v>
-      </c>
-      <c r="T3">
-        <v>2</v>
-      </c>
-      <c r="U3">
-        <v>3</v>
-      </c>
-      <c r="V3">
-        <v>2</v>
-      </c>
-      <c r="W3">
-        <v>3</v>
-      </c>
-      <c r="X3">
-        <v>2</v>
-      </c>
-      <c r="Y3">
-        <v>3</v>
-      </c>
-      <c r="Z3">
+        <v/>
+      </c>
+      <c r="R3" t="n">
+        <v>2</v>
+      </c>
+      <c r="S3" t="n">
+        <v>3</v>
+      </c>
+      <c r="T3" t="n">
+        <v>2</v>
+      </c>
+      <c r="U3" t="n">
+        <v>3</v>
+      </c>
+      <c r="V3" t="n">
+        <v>2</v>
+      </c>
+      <c r="W3" t="n">
+        <v>3</v>
+      </c>
+      <c r="X3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z3" t="n">
         <v>2</v>
       </c>
       <c r="AA3" s="3">
         <f>SUM(R3:Z3)</f>
-        <v>22</v>
+        <v/>
       </c>
       <c r="AB3" s="1" t="s">
         <v>58</v>
@@ -1196,50 +1196,50 @@
       </c>
       <c r="AK3" s="3">
         <f>ROUND(IF(AB3="+",1,IF(AB3="+.",1,IF(AB3="+-",0.8,IF(AB3="+/2",0.5,IF(AB3="-+",0.1,IF(AB3="-.",0,IF(AB3="-",0,IF(AB3="0",0,IF(AB3="",0,"?")))))))))+IF(AC3="+",1,IF(AC3="+.",1,IF(AC3="+-",0.8,IF(AC3="+/2",0.5,IF(AC3="-+",0.1,IF(AC3="-.",0,IF(AC3="-",0,IF(AC3="0",0,IF(AC3="",0,"?")))))))))+IF(AD3="+",1,IF(AD3="+.",1,IF(AD3="+-",0.8,IF(AD3="+/2",0.5,IF(AD3="-+",0.1,IF(AD3="-.",0,IF(AD3="-",0,IF(AD3="0",0,IF(AD3="",0,"?")))))))))+IF(AE3="+",1,IF(AE3="+.",1,IF(AE3="+-",0.8,IF(AE3="+/2",0.5,IF(AE3="-+",0.1,IF(AE3="-.",0,IF(AE3="-",0,IF(AE3="0",0,IF(AE3="",0,"?")))))))))+IF(AF3="+",1,IF(AF3="+.",1,IF(AF3="+-",0.8,IF(AF3="+/2",0.5,IF(AF3="-+",0.1,IF(AF3="-.",0,IF(AF3="-",0,IF(AF3="0",0,IF(AF3="",0,"?")))))))))+IF(AG3="+",1,IF(AG3="+.",1,IF(AG3="+-",0.8,IF(AG3="+/2",0.5,IF(AG3="-+",0.1,IF(AG3="-.",0,IF(AG3="-",0,IF(AG3="0",0,IF(AG3="",0,"?")))))))))+IF(AH3="+",1,IF(AH3="+.",1,IF(AH3="+-",0.8,IF(AH3="+/2",0.5,IF(AH3="-+",0.1,IF(AH3="-.",0,IF(AH3="-",0,IF(AH3="0",0,IF(AH3="",0,"?")))))))))+IF(AI3="+",1,IF(AI3="+.",1,IF(AI3="+-",0.8,IF(AI3="+/2",0.5,IF(AI3="-+",0.1,IF(AI3="-.",0,IF(AI3="-",0,IF(AI3="0",0,IF(AI3="",0,"?")))))))))+IF(AJ3="+",1,IF(AJ3="+.",1,IF(AJ3="+-",0.8,IF(AJ3="+/2",0.5,IF(AJ3="-+",0.1,IF(AJ3="-.",0,IF(AJ3="-",0,IF(AJ3="0",0,IF(AJ3="",0,"?"))))))))),2)</f>
-        <v>3.5</v>
+        <v/>
       </c>
       <c r="AL3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AB3="+",1,IF(AB3="+.",1,IF(AB3="+-",0.8,IF(AB3="+/2",0.5,IF(AB3="-+",0.1,IF(AB3="-.",0,IF(AB3="-",0,IF(AB3="0",0,IF(AB3="",0,"?")))))))))*R3,2)</f>
+        <v/>
       </c>
       <c r="AM3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AC3="+",1,IF(AC3="+.",1,IF(AC3="+-",0.8,IF(AC3="+/2",0.5,IF(AC3="-+",0.1,IF(AC3="-.",0,IF(AC3="-",0,IF(AC3="0",0,IF(AC3="",0,"?")))))))))*S3,2)</f>
+        <v/>
       </c>
       <c r="AN3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>ROUND(IF(AD3="+",1,IF(AD3="+.",1,IF(AD3="+-",0.8,IF(AD3="+/2",0.5,IF(AD3="-+",0.1,IF(AD3="-.",0,IF(AD3="-",0,IF(AD3="0",0,IF(AD3="",0,"?")))))))))*T3,2)</f>
+        <v/>
       </c>
       <c r="AO3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>ROUND(IF(AE3="+",1,IF(AE3="+.",1,IF(AE3="+-",0.8,IF(AE3="+/2",0.5,IF(AE3="-+",0.1,IF(AE3="-.",0,IF(AE3="-",0,IF(AE3="0",0,IF(AE3="",0,"?")))))))))*U3,2)</f>
+        <v/>
       </c>
       <c r="AP3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>ROUND(IF(AF3="+",1,IF(AF3="+.",1,IF(AF3="+-",0.8,IF(AF3="+/2",0.5,IF(AF3="-+",0.1,IF(AF3="-.",0,IF(AF3="-",0,IF(AF3="0",0,IF(AF3="",0,"?")))))))))*V3,2)</f>
+        <v/>
       </c>
       <c r="AQ3">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
+        <f>ROUND(IF(AG3="+",1,IF(AG3="+.",1,IF(AG3="+-",0.8,IF(AG3="+/2",0.5,IF(AG3="-+",0.1,IF(AG3="-.",0,IF(AG3="-",0,IF(AG3="0",0,IF(AG3="",0,"?")))))))))*W3,2)</f>
+        <v/>
       </c>
       <c r="AR3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AH3="+",1,IF(AH3="+.",1,IF(AH3="+-",0.8,IF(AH3="+/2",0.5,IF(AH3="-+",0.1,IF(AH3="-.",0,IF(AH3="-",0,IF(AH3="0",0,IF(AH3="",0,"?")))))))))*X3,2)</f>
+        <v/>
       </c>
       <c r="AS3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AI3="+",1,IF(AI3="+.",1,IF(AI3="+-",0.8,IF(AI3="+/2",0.5,IF(AI3="-+",0.1,IF(AI3="-.",0,IF(AI3="-",0,IF(AI3="0",0,IF(AI3="",0,"?")))))))))*Y3,2)</f>
+        <v/>
       </c>
       <c r="AT3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AJ3="+",1,IF(AJ3="+.",1,IF(AJ3="+-",0.8,IF(AJ3="+/2",0.5,IF(AJ3="-+",0.1,IF(AJ3="-.",0,IF(AJ3="-",0,IF(AJ3="0",0,IF(AJ3="",0,"?")))))))))*Z3,2)</f>
+        <v/>
       </c>
       <c r="AU3" s="3">
         <f>SUM(AL3:AT3)</f>
-        <v>8.5</v>
+        <v/>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1255,13 +1255,13 @@
       <c r="E4" t="s">
         <v>70</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="n">
         <v>305</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="n">
         <v>123</v>
       </c>
-      <c r="H4">
+      <c r="H4" t="n">
         <v>2003</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -1270,13 +1270,13 @@
       <c r="J4" t="s">
         <v>52</v>
       </c>
-      <c r="L4" t="str">
+      <c r="L4">
         <f>"Собеседования в 7-й математический класс 179-й школы"</f>
-        <v>Собеседования в 7-й математический класс 179-й школы</v>
-      </c>
-      <c r="M4" t="str">
+        <v/>
+      </c>
+      <c r="M4">
         <f>"|"</f>
-        <v>|</v>
+        <v/>
       </c>
       <c r="N4" t="s">
         <v>53</v>
@@ -1287,40 +1287,40 @@
       <c r="P4" t="s">
         <v>55</v>
       </c>
-      <c r="Q4" t="str">
+      <c r="Q4">
         <f>"|"</f>
-        <v>|</v>
-      </c>
-      <c r="R4">
-        <v>2</v>
-      </c>
-      <c r="S4">
-        <v>3</v>
-      </c>
-      <c r="T4">
-        <v>2</v>
-      </c>
-      <c r="U4">
-        <v>3</v>
-      </c>
-      <c r="V4">
-        <v>2</v>
-      </c>
-      <c r="W4">
-        <v>3</v>
-      </c>
-      <c r="X4">
-        <v>2</v>
-      </c>
-      <c r="Y4">
-        <v>3</v>
-      </c>
-      <c r="Z4">
+        <v/>
+      </c>
+      <c r="R4" t="n">
+        <v>2</v>
+      </c>
+      <c r="S4" t="n">
+        <v>3</v>
+      </c>
+      <c r="T4" t="n">
+        <v>2</v>
+      </c>
+      <c r="U4" t="n">
+        <v>3</v>
+      </c>
+      <c r="V4" t="n">
+        <v>2</v>
+      </c>
+      <c r="W4" t="n">
+        <v>3</v>
+      </c>
+      <c r="X4" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z4" t="n">
         <v>2</v>
       </c>
       <c r="AA4" s="3">
         <f>SUM(R4:Z4)</f>
-        <v>22</v>
+        <v/>
       </c>
       <c r="AB4" s="1" t="s">
         <v>58</v>
@@ -1345,50 +1345,53 @@
       </c>
       <c r="AK4" s="3">
         <f>ROUND(IF(AB4="+",1,IF(AB4="+.",1,IF(AB4="+-",0.8,IF(AB4="+/2",0.5,IF(AB4="-+",0.1,IF(AB4="-.",0,IF(AB4="-",0,IF(AB4="0",0,IF(AB4="",0,"?")))))))))+IF(AC4="+",1,IF(AC4="+.",1,IF(AC4="+-",0.8,IF(AC4="+/2",0.5,IF(AC4="-+",0.1,IF(AC4="-.",0,IF(AC4="-",0,IF(AC4="0",0,IF(AC4="",0,"?")))))))))+IF(AD4="+",1,IF(AD4="+.",1,IF(AD4="+-",0.8,IF(AD4="+/2",0.5,IF(AD4="-+",0.1,IF(AD4="-.",0,IF(AD4="-",0,IF(AD4="0",0,IF(AD4="",0,"?")))))))))+IF(AE4="+",1,IF(AE4="+.",1,IF(AE4="+-",0.8,IF(AE4="+/2",0.5,IF(AE4="-+",0.1,IF(AE4="-.",0,IF(AE4="-",0,IF(AE4="0",0,IF(AE4="",0,"?")))))))))+IF(AF4="+",1,IF(AF4="+.",1,IF(AF4="+-",0.8,IF(AF4="+/2",0.5,IF(AF4="-+",0.1,IF(AF4="-.",0,IF(AF4="-",0,IF(AF4="0",0,IF(AF4="",0,"?")))))))))+IF(AG4="+",1,IF(AG4="+.",1,IF(AG4="+-",0.8,IF(AG4="+/2",0.5,IF(AG4="-+",0.1,IF(AG4="-.",0,IF(AG4="-",0,IF(AG4="0",0,IF(AG4="",0,"?")))))))))+IF(AH4="+",1,IF(AH4="+.",1,IF(AH4="+-",0.8,IF(AH4="+/2",0.5,IF(AH4="-+",0.1,IF(AH4="-.",0,IF(AH4="-",0,IF(AH4="0",0,IF(AH4="",0,"?")))))))))+IF(AI4="+",1,IF(AI4="+.",1,IF(AI4="+-",0.8,IF(AI4="+/2",0.5,IF(AI4="-+",0.1,IF(AI4="-.",0,IF(AI4="-",0,IF(AI4="0",0,IF(AI4="",0,"?")))))))))+IF(AJ4="+",1,IF(AJ4="+.",1,IF(AJ4="+-",0.8,IF(AJ4="+/2",0.5,IF(AJ4="-+",0.1,IF(AJ4="-.",0,IF(AJ4="-",0,IF(AJ4="0",0,IF(AJ4="",0,"?"))))))))),2)</f>
-        <v>5.0999999999999996</v>
+        <v/>
       </c>
       <c r="AL4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AB4="+",1,IF(AB4="+.",1,IF(AB4="+-",0.8,IF(AB4="+/2",0.5,IF(AB4="-+",0.1,IF(AB4="-.",0,IF(AB4="-",0,IF(AB4="0",0,IF(AB4="",0,"?")))))))))*R4,2)</f>
+        <v/>
       </c>
       <c r="AM4">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>ROUND(IF(AC4="+",1,IF(AC4="+.",1,IF(AC4="+-",0.8,IF(AC4="+/2",0.5,IF(AC4="-+",0.1,IF(AC4="-.",0,IF(AC4="-",0,IF(AC4="0",0,IF(AC4="",0,"?")))))))))*S4,2)</f>
+        <v/>
       </c>
       <c r="AN4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>ROUND(IF(AD4="+",1,IF(AD4="+.",1,IF(AD4="+-",0.8,IF(AD4="+/2",0.5,IF(AD4="-+",0.1,IF(AD4="-.",0,IF(AD4="-",0,IF(AD4="0",0,IF(AD4="",0,"?")))))))))*T4,2)</f>
+        <v/>
       </c>
       <c r="AO4">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>ROUND(IF(AE4="+",1,IF(AE4="+.",1,IF(AE4="+-",0.8,IF(AE4="+/2",0.5,IF(AE4="-+",0.1,IF(AE4="-.",0,IF(AE4="-",0,IF(AE4="0",0,IF(AE4="",0,"?")))))))))*U4,2)</f>
+        <v/>
       </c>
       <c r="AP4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>ROUND(IF(AF4="+",1,IF(AF4="+.",1,IF(AF4="+-",0.8,IF(AF4="+/2",0.5,IF(AF4="-+",0.1,IF(AF4="-.",0,IF(AF4="-",0,IF(AF4="0",0,IF(AF4="",0,"?")))))))))*V4,2)</f>
+        <v/>
       </c>
       <c r="AQ4">
-        <f t="shared" si="0"/>
-        <v>0.3</v>
+        <f>ROUND(IF(AG4="+",1,IF(AG4="+.",1,IF(AG4="+-",0.8,IF(AG4="+/2",0.5,IF(AG4="-+",0.1,IF(AG4="-.",0,IF(AG4="-",0,IF(AG4="0",0,IF(AG4="",0,"?")))))))))*W4,2)</f>
+        <v/>
       </c>
       <c r="AR4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>ROUND(IF(AH4="+",1,IF(AH4="+.",1,IF(AH4="+-",0.8,IF(AH4="+/2",0.5,IF(AH4="-+",0.1,IF(AH4="-.",0,IF(AH4="-",0,IF(AH4="0",0,IF(AH4="",0,"?")))))))))*X4,2)</f>
+        <v/>
       </c>
       <c r="AS4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AI4="+",1,IF(AI4="+.",1,IF(AI4="+-",0.8,IF(AI4="+/2",0.5,IF(AI4="-+",0.1,IF(AI4="-.",0,IF(AI4="-",0,IF(AI4="0",0,IF(AI4="",0,"?")))))))))*Y4,2)</f>
+        <v/>
       </c>
       <c r="AT4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AJ4="+",1,IF(AJ4="+.",1,IF(AJ4="+-",0.8,IF(AJ4="+/2",0.5,IF(AJ4="-+",0.1,IF(AJ4="-.",0,IF(AJ4="-",0,IF(AJ4="0",0,IF(AJ4="",0,"?")))))))))*Z4,2)</f>
+        <v/>
       </c>
       <c r="AU4" s="3">
         <f>SUM(AL4:AT4)</f>
-        <v>12.3</v>
+        <v/>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
       <c r="B5" t="s">
         <v>74</v>
       </c>
@@ -1401,13 +1404,13 @@
       <c r="E5" t="s">
         <v>76</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="n">
         <v>207</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="n">
         <v>432</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="n">
         <v>2004</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -1419,13 +1422,13 @@
       <c r="K5" t="s">
         <v>10</v>
       </c>
-      <c r="L5" t="str">
+      <c r="L5">
         <f>"Собеседования в 7-й математический класс 179-й школы"</f>
-        <v>Собеседования в 7-й математический класс 179-й школы</v>
-      </c>
-      <c r="M5" t="str">
+        <v/>
+      </c>
+      <c r="M5">
         <f>"|"</f>
-        <v>|</v>
+        <v/>
       </c>
       <c r="N5" t="s">
         <v>53</v>
@@ -1436,40 +1439,40 @@
       <c r="P5" t="s">
         <v>55</v>
       </c>
-      <c r="Q5" t="str">
+      <c r="Q5">
         <f>"|"</f>
-        <v>|</v>
-      </c>
-      <c r="R5">
-        <v>2</v>
-      </c>
-      <c r="S5">
-        <v>3</v>
-      </c>
-      <c r="T5">
-        <v>2</v>
-      </c>
-      <c r="U5">
-        <v>3</v>
-      </c>
-      <c r="V5">
-        <v>2</v>
-      </c>
-      <c r="W5">
-        <v>3</v>
-      </c>
-      <c r="X5">
-        <v>2</v>
-      </c>
-      <c r="Y5">
-        <v>3</v>
-      </c>
-      <c r="Z5">
+        <v/>
+      </c>
+      <c r="R5" t="n">
+        <v>2</v>
+      </c>
+      <c r="S5" t="n">
+        <v>3</v>
+      </c>
+      <c r="T5" t="n">
+        <v>2</v>
+      </c>
+      <c r="U5" t="n">
+        <v>3</v>
+      </c>
+      <c r="V5" t="n">
+        <v>2</v>
+      </c>
+      <c r="W5" t="n">
+        <v>3</v>
+      </c>
+      <c r="X5" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z5" t="n">
         <v>2</v>
       </c>
       <c r="AA5" s="3">
         <f>SUM(R5:Z5)</f>
-        <v>22</v>
+        <v/>
       </c>
       <c r="AB5" s="1" t="s">
         <v>56</v>
@@ -1494,47 +1497,47 @@
       </c>
       <c r="AK5" s="3">
         <f>ROUND(IF(AB5="+",1,IF(AB5="+.",1,IF(AB5="+-",0.8,IF(AB5="+/2",0.5,IF(AB5="-+",0.1,IF(AB5="-.",0,IF(AB5="-",0,IF(AB5="0",0,IF(AB5="",0,"?")))))))))+IF(AC5="+",1,IF(AC5="+.",1,IF(AC5="+-",0.8,IF(AC5="+/2",0.5,IF(AC5="-+",0.1,IF(AC5="-.",0,IF(AC5="-",0,IF(AC5="0",0,IF(AC5="",0,"?")))))))))+IF(AD5="+",1,IF(AD5="+.",1,IF(AD5="+-",0.8,IF(AD5="+/2",0.5,IF(AD5="-+",0.1,IF(AD5="-.",0,IF(AD5="-",0,IF(AD5="0",0,IF(AD5="",0,"?")))))))))+IF(AE5="+",1,IF(AE5="+.",1,IF(AE5="+-",0.8,IF(AE5="+/2",0.5,IF(AE5="-+",0.1,IF(AE5="-.",0,IF(AE5="-",0,IF(AE5="0",0,IF(AE5="",0,"?")))))))))+IF(AF5="+",1,IF(AF5="+.",1,IF(AF5="+-",0.8,IF(AF5="+/2",0.5,IF(AF5="-+",0.1,IF(AF5="-.",0,IF(AF5="-",0,IF(AF5="0",0,IF(AF5="",0,"?")))))))))+IF(AG5="+",1,IF(AG5="+.",1,IF(AG5="+-",0.8,IF(AG5="+/2",0.5,IF(AG5="-+",0.1,IF(AG5="-.",0,IF(AG5="-",0,IF(AG5="0",0,IF(AG5="",0,"?")))))))))+IF(AH5="+",1,IF(AH5="+.",1,IF(AH5="+-",0.8,IF(AH5="+/2",0.5,IF(AH5="-+",0.1,IF(AH5="-.",0,IF(AH5="-",0,IF(AH5="0",0,IF(AH5="",0,"?")))))))))+IF(AI5="+",1,IF(AI5="+.",1,IF(AI5="+-",0.8,IF(AI5="+/2",0.5,IF(AI5="-+",0.1,IF(AI5="-.",0,IF(AI5="-",0,IF(AI5="0",0,IF(AI5="",0,"?")))))))))+IF(AJ5="+",1,IF(AJ5="+.",1,IF(AJ5="+-",0.8,IF(AJ5="+/2",0.5,IF(AJ5="-+",0.1,IF(AJ5="-.",0,IF(AJ5="-",0,IF(AJ5="0",0,IF(AJ5="",0,"?"))))))))),2)</f>
-        <v>3</v>
+        <v/>
       </c>
       <c r="AL5">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>ROUND(IF(AB5="+",1,IF(AB5="+.",1,IF(AB5="+-",0.8,IF(AB5="+/2",0.5,IF(AB5="-+",0.1,IF(AB5="-.",0,IF(AB5="-",0,IF(AB5="0",0,IF(AB5="",0,"?")))))))))*R5,2)</f>
+        <v/>
       </c>
       <c r="AM5">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>ROUND(IF(AC5="+",1,IF(AC5="+.",1,IF(AC5="+-",0.8,IF(AC5="+/2",0.5,IF(AC5="-+",0.1,IF(AC5="-.",0,IF(AC5="-",0,IF(AC5="0",0,IF(AC5="",0,"?")))))))))*S5,2)</f>
+        <v/>
       </c>
       <c r="AN5">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>ROUND(IF(AD5="+",1,IF(AD5="+.",1,IF(AD5="+-",0.8,IF(AD5="+/2",0.5,IF(AD5="-+",0.1,IF(AD5="-.",0,IF(AD5="-",0,IF(AD5="0",0,IF(AD5="",0,"?")))))))))*T5,2)</f>
+        <v/>
       </c>
       <c r="AO5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AE5="+",1,IF(AE5="+.",1,IF(AE5="+-",0.8,IF(AE5="+/2",0.5,IF(AE5="-+",0.1,IF(AE5="-.",0,IF(AE5="-",0,IF(AE5="0",0,IF(AE5="",0,"?")))))))))*U5,2)</f>
+        <v/>
       </c>
       <c r="AP5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AF5="+",1,IF(AF5="+.",1,IF(AF5="+-",0.8,IF(AF5="+/2",0.5,IF(AF5="-+",0.1,IF(AF5="-.",0,IF(AF5="-",0,IF(AF5="0",0,IF(AF5="",0,"?")))))))))*V5,2)</f>
+        <v/>
       </c>
       <c r="AQ5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AG5="+",1,IF(AG5="+.",1,IF(AG5="+-",0.8,IF(AG5="+/2",0.5,IF(AG5="-+",0.1,IF(AG5="-.",0,IF(AG5="-",0,IF(AG5="0",0,IF(AG5="",0,"?")))))))))*W5,2)</f>
+        <v/>
       </c>
       <c r="AR5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AH5="+",1,IF(AH5="+.",1,IF(AH5="+-",0.8,IF(AH5="+/2",0.5,IF(AH5="-+",0.1,IF(AH5="-.",0,IF(AH5="-",0,IF(AH5="0",0,IF(AH5="",0,"?")))))))))*X5,2)</f>
+        <v/>
       </c>
       <c r="AS5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AI5="+",1,IF(AI5="+.",1,IF(AI5="+-",0.8,IF(AI5="+/2",0.5,IF(AI5="-+",0.1,IF(AI5="-.",0,IF(AI5="-",0,IF(AI5="0",0,IF(AI5="",0,"?")))))))))*Y5,2)</f>
+        <v/>
       </c>
       <c r="AT5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AJ5="+",1,IF(AJ5="+.",1,IF(AJ5="+-",0.8,IF(AJ5="+/2",0.5,IF(AJ5="-+",0.1,IF(AJ5="-.",0,IF(AJ5="-",0,IF(AJ5="0",0,IF(AJ5="",0,"?")))))))))*Z5,2)</f>
+        <v/>
       </c>
       <c r="AU5" s="3">
         <f>SUM(AL5:AT5)</f>
-        <v>7</v>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -1544,8 +1547,8 @@
     <hyperlink ref="I4" r:id="rId3"/>
     <hyperlink ref="I5" r:id="rId4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <tableParts count="1">
     <tablePart r:id="rId5"/>
   </tableParts>

</xml_diff>

<commit_message>
Lot's of refactoring and improvements
</commit_message>
<xml_diff>
--- a/send_list.xlsx
+++ b/send_list.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="525" windowWidth="19815" windowHeight="6600"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="80">
   <si>
     <t>ok</t>
   </si>
@@ -259,38 +259,39 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color theme="10"/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -312,23 +313,23 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Обычный" xfId="0"/>
+    <cellStyle builtinId="8" name="Гиперссылка" xfId="1"/>
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -337,7 +338,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -348,34 +349,34 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -384,17 +385,12 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица2" displayName="Таблица2" ref="A1:AU5" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Таблица2" headerRowCount="1" id="1" name="Таблица2" ref="A1:AU5" totalsRowShown="0">
   <autoFilter ref="A1:AU5"/>
   <tableColumns count="47">
     <tableColumn id="1" name="ok"/>
@@ -405,7 +401,7 @@
     <tableColumn id="6" name="Ауд"/>
     <tableColumn id="7" name="Школа"/>
     <tableColumn id="8" name="Год р."/>
-    <tableColumn id="9" name="email" dataCellStyle="Гиперссылка"/>
+    <tableColumn dataCellStyle="Гиперссылка" id="9" name="email"/>
     <tableColumn id="10" name="пол"/>
     <tableColumn id="11" name="а"/>
     <tableColumn id="12" name="subject">
@@ -429,22 +425,22 @@
     <tableColumn id="24" name="mx7"/>
     <tableColumn id="25" name="mx8"/>
     <tableColumn id="26" name="mx9"/>
-    <tableColumn id="27" name="mxtot" dataDxfId="12">
+    <tableColumn dataDxfId="12" id="27" name="mxtot">
       <calculatedColumnFormula>SUM(R2:Z2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" name="pl1" dataDxfId="11"/>
-    <tableColumn id="29" name="pl2" dataDxfId="10"/>
-    <tableColumn id="30" name="pl3" dataDxfId="9"/>
-    <tableColumn id="31" name="pl4" dataDxfId="8"/>
-    <tableColumn id="32" name="pl5" dataDxfId="7"/>
-    <tableColumn id="33" name="pl6" dataDxfId="6"/>
-    <tableColumn id="34" name="pl7" dataDxfId="5"/>
-    <tableColumn id="35" name="pl8" dataDxfId="4"/>
-    <tableColumn id="36" name="pl9" dataDxfId="3"/>
-    <tableColumn id="37" name="pltot" dataDxfId="2">
+    <tableColumn dataDxfId="11" id="28" name="pl1"/>
+    <tableColumn dataDxfId="10" id="29" name="pl2"/>
+    <tableColumn dataDxfId="9" id="30" name="pl3"/>
+    <tableColumn dataDxfId="8" id="31" name="pl4"/>
+    <tableColumn dataDxfId="7" id="32" name="pl5"/>
+    <tableColumn dataDxfId="6" id="33" name="pl6"/>
+    <tableColumn dataDxfId="5" id="34" name="pl7"/>
+    <tableColumn dataDxfId="4" id="35" name="pl8"/>
+    <tableColumn dataDxfId="3" id="36" name="pl9"/>
+    <tableColumn dataDxfId="2" id="37" name="pltot">
       <calculatedColumnFormula>ROUND(IF(AB2="+",1,IF(AB2="+.",1,IF(AB2="+-",0.8,IF(AB2="+/2",0.5,IF(AB2="-+",0.1,IF(AB2="-.",0,IF(AB2="-",0,IF(AB2="0",0,IF(AB2="",0,"?")))))))))+IF(AC2="+",1,IF(AC2="+.",1,IF(AC2="+-",0.8,IF(AC2="+/2",0.5,IF(AC2="-+",0.1,IF(AC2="-.",0,IF(AC2="-",0,IF(AC2="0",0,IF(AC2="",0,"?")))))))))+IF(AD2="+",1,IF(AD2="+.",1,IF(AD2="+-",0.8,IF(AD2="+/2",0.5,IF(AD2="-+",0.1,IF(AD2="-.",0,IF(AD2="-",0,IF(AD2="0",0,IF(AD2="",0,"?")))))))))+IF(AE2="+",1,IF(AE2="+.",1,IF(AE2="+-",0.8,IF(AE2="+/2",0.5,IF(AE2="-+",0.1,IF(AE2="-.",0,IF(AE2="-",0,IF(AE2="0",0,IF(AE2="",0,"?")))))))))+IF(AF2="+",1,IF(AF2="+.",1,IF(AF2="+-",0.8,IF(AF2="+/2",0.5,IF(AF2="-+",0.1,IF(AF2="-.",0,IF(AF2="-",0,IF(AF2="0",0,IF(AF2="",0,"?")))))))))+IF(AG2="+",1,IF(AG2="+.",1,IF(AG2="+-",0.8,IF(AG2="+/2",0.5,IF(AG2="-+",0.1,IF(AG2="-.",0,IF(AG2="-",0,IF(AG2="0",0,IF(AG2="",0,"?")))))))))+IF(AH2="+",1,IF(AH2="+.",1,IF(AH2="+-",0.8,IF(AH2="+/2",0.5,IF(AH2="-+",0.1,IF(AH2="-.",0,IF(AH2="-",0,IF(AH2="0",0,IF(AH2="",0,"?")))))))))+IF(AI2="+",1,IF(AI2="+.",1,IF(AI2="+-",0.8,IF(AI2="+/2",0.5,IF(AI2="-+",0.1,IF(AI2="-.",0,IF(AI2="-",0,IF(AI2="0",0,IF(AI2="",0,"?")))))))))+IF(AJ2="+",1,IF(AJ2="+.",1,IF(AJ2="+-",0.8,IF(AJ2="+/2",0.5,IF(AJ2="-+",0.1,IF(AJ2="-.",0,IF(AJ2="-",0,IF(AJ2="0",0,IF(AJ2="",0,"?"))))))))),2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" name="bl1" dataDxfId="1">
+    <tableColumn dataDxfId="1" id="38" name="bl1">
       <calculatedColumnFormula>ROUND(IF(AB2="+",1,IF(AB2="+.",1,IF(AB2="+-",0.8,IF(AB2="+/2",0.5,IF(AB2="-+",0.1,IF(AB2="-.",0,IF(AB2="-",0,IF(AB2="0",0,IF(AB2="",0,"?")))))))))*R2,2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="39" name="bl2">
@@ -471,11 +467,11 @@
     <tableColumn id="46" name="bl9">
       <calculatedColumnFormula>ROUND(IF(AJ2="+",1,IF(AJ2="+.",1,IF(AJ2="+-",0.8,IF(AJ2="+/2",0.5,IF(AJ2="-+",0.1,IF(AJ2="-.",0,IF(AJ2="-",0,IF(AJ2="0",0,IF(AJ2="",0,"?")))))))))*Z2,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="47" name="bltot" dataDxfId="0">
+    <tableColumn dataDxfId="0" id="47" name="bltot">
       <calculatedColumnFormula>SUM(AL2:AT2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
@@ -765,43 +761,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:AU5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" customWidth="1"/>
-    <col min="11" max="11" width="4.140625" customWidth="1"/>
-    <col min="12" max="12" width="54.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.140625" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" customWidth="1"/>
-    <col min="15" max="15" width="41" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.140625" customWidth="1"/>
-    <col min="18" max="26" width="6.85546875" customWidth="1"/>
-    <col min="27" max="27" width="8.42578125" style="3" customWidth="1"/>
-    <col min="28" max="36" width="5.85546875" style="1" customWidth="1"/>
-    <col min="37" max="37" width="7.42578125" style="3" customWidth="1"/>
-    <col min="38" max="38" width="5.85546875" customWidth="1"/>
-    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="40" max="46" width="5.85546875" customWidth="1"/>
-    <col min="47" max="47" width="7.42578125" style="3" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="5.28515625"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="5.5703125"/>
+    <col customWidth="1" max="3" min="3" width="18"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="13.5703125"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" width="10.42578125"/>
+    <col customWidth="1" max="6" min="6" width="6.5703125"/>
+    <col customWidth="1" max="7" min="7" width="9.28515625"/>
+    <col customWidth="1" max="8" min="8" width="8.42578125"/>
+    <col bestFit="1" customWidth="1" max="9" min="9" width="17"/>
+    <col customWidth="1" max="10" min="10" width="6.5703125"/>
+    <col customWidth="1" max="11" min="11" width="4.140625"/>
+    <col bestFit="1" customWidth="1" max="12" min="12" width="54.140625"/>
+    <col customWidth="1" max="13" min="13" width="4.140625"/>
+    <col customWidth="1" max="14" min="14" width="9.5703125"/>
+    <col bestFit="1" customWidth="1" max="15" min="15" width="41"/>
+    <col bestFit="1" customWidth="1" max="16" min="16" width="17.85546875"/>
+    <col customWidth="1" max="17" min="17" width="5.140625"/>
+    <col customWidth="1" max="26" min="18" width="6.85546875"/>
+    <col customWidth="1" max="27" min="27" style="3" width="8.42578125"/>
+    <col customWidth="1" max="36" min="28" style="1" width="5.85546875"/>
+    <col customWidth="1" max="37" min="37" style="3" width="7.42578125"/>
+    <col customWidth="1" max="38" min="38" width="5.85546875"/>
+    <col bestFit="1" customWidth="1" max="39" min="39" width="7.42578125"/>
+    <col customWidth="1" max="46" min="40" width="5.85546875"/>
+    <col customWidth="1" max="47" min="47" style="3" width="7.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -944,7 +944,10 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" t="s">
         <v>47</v>
       </c>
@@ -957,13 +960,13 @@
       <c r="E2" t="s">
         <v>50</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="n">
         <v>305</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="n">
         <v>123</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="n">
         <v>2001</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -972,13 +975,13 @@
       <c r="J2" t="s">
         <v>52</v>
       </c>
-      <c r="L2" t="str">
+      <c r="L2">
         <f>"Собеседования в 7-й математический класс 179-й школы"</f>
-        <v>Собеседования в 7-й математический класс 179-й школы</v>
-      </c>
-      <c r="M2" t="str">
+        <v/>
+      </c>
+      <c r="M2">
         <f>"|"</f>
-        <v>|</v>
+        <v/>
       </c>
       <c r="N2" t="s">
         <v>53</v>
@@ -989,40 +992,40 @@
       <c r="P2" t="s">
         <v>55</v>
       </c>
-      <c r="Q2" t="str">
+      <c r="Q2">
         <f>"|"</f>
-        <v>|</v>
-      </c>
-      <c r="R2">
-        <v>2</v>
-      </c>
-      <c r="S2">
-        <v>3</v>
-      </c>
-      <c r="T2">
-        <v>2</v>
-      </c>
-      <c r="U2">
-        <v>3</v>
-      </c>
-      <c r="V2">
-        <v>2</v>
-      </c>
-      <c r="W2">
-        <v>3</v>
-      </c>
-      <c r="X2">
-        <v>2</v>
-      </c>
-      <c r="Y2">
-        <v>3</v>
-      </c>
-      <c r="Z2">
+        <v/>
+      </c>
+      <c r="R2" t="n">
+        <v>2</v>
+      </c>
+      <c r="S2" t="n">
+        <v>3</v>
+      </c>
+      <c r="T2" t="n">
+        <v>2</v>
+      </c>
+      <c r="U2" t="n">
+        <v>3</v>
+      </c>
+      <c r="V2" t="n">
+        <v>2</v>
+      </c>
+      <c r="W2" t="n">
+        <v>3</v>
+      </c>
+      <c r="X2" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z2" t="n">
         <v>2</v>
       </c>
       <c r="AA2" s="3">
         <f>SUM(R2:Z2)</f>
-        <v>22</v>
+        <v/>
       </c>
       <c r="AB2" s="1" t="s">
         <v>56</v>
@@ -1047,50 +1050,50 @@
       </c>
       <c r="AK2" s="3">
         <f>ROUND(IF(AB2="+",1,IF(AB2="+.",1,IF(AB2="+-",0.8,IF(AB2="+/2",0.5,IF(AB2="-+",0.1,IF(AB2="-.",0,IF(AB2="-",0,IF(AB2="0",0,IF(AB2="",0,"?")))))))))+IF(AC2="+",1,IF(AC2="+.",1,IF(AC2="+-",0.8,IF(AC2="+/2",0.5,IF(AC2="-+",0.1,IF(AC2="-.",0,IF(AC2="-",0,IF(AC2="0",0,IF(AC2="",0,"?")))))))))+IF(AD2="+",1,IF(AD2="+.",1,IF(AD2="+-",0.8,IF(AD2="+/2",0.5,IF(AD2="-+",0.1,IF(AD2="-.",0,IF(AD2="-",0,IF(AD2="0",0,IF(AD2="",0,"?")))))))))+IF(AE2="+",1,IF(AE2="+.",1,IF(AE2="+-",0.8,IF(AE2="+/2",0.5,IF(AE2="-+",0.1,IF(AE2="-.",0,IF(AE2="-",0,IF(AE2="0",0,IF(AE2="",0,"?")))))))))+IF(AF2="+",1,IF(AF2="+.",1,IF(AF2="+-",0.8,IF(AF2="+/2",0.5,IF(AF2="-+",0.1,IF(AF2="-.",0,IF(AF2="-",0,IF(AF2="0",0,IF(AF2="",0,"?")))))))))+IF(AG2="+",1,IF(AG2="+.",1,IF(AG2="+-",0.8,IF(AG2="+/2",0.5,IF(AG2="-+",0.1,IF(AG2="-.",0,IF(AG2="-",0,IF(AG2="0",0,IF(AG2="",0,"?")))))))))+IF(AH2="+",1,IF(AH2="+.",1,IF(AH2="+-",0.8,IF(AH2="+/2",0.5,IF(AH2="-+",0.1,IF(AH2="-.",0,IF(AH2="-",0,IF(AH2="0",0,IF(AH2="",0,"?")))))))))+IF(AI2="+",1,IF(AI2="+.",1,IF(AI2="+-",0.8,IF(AI2="+/2",0.5,IF(AI2="-+",0.1,IF(AI2="-.",0,IF(AI2="-",0,IF(AI2="0",0,IF(AI2="",0,"?")))))))))+IF(AJ2="+",1,IF(AJ2="+.",1,IF(AJ2="+-",0.8,IF(AJ2="+/2",0.5,IF(AJ2="-+",0.1,IF(AJ2="-.",0,IF(AJ2="-",0,IF(AJ2="0",0,IF(AJ2="",0,"?"))))))))),2)</f>
-        <v>2.8</v>
+        <v/>
       </c>
       <c r="AL2">
-        <f t="shared" ref="AL2:AT5" si="0">ROUND(IF(AB2="+",1,IF(AB2="+.",1,IF(AB2="+-",0.8,IF(AB2="+/2",0.5,IF(AB2="-+",0.1,IF(AB2="-.",0,IF(AB2="-",0,IF(AB2="0",0,IF(AB2="",0,"?")))))))))*R2,2)</f>
-        <v>2</v>
+        <f>ROUND(IF(AB2="+",1,IF(AB2="+.",1,IF(AB2="+-",0.8,IF(AB2="+/2",0.5,IF(AB2="-+",0.1,IF(AB2="-.",0,IF(AB2="-",0,IF(AB2="0",0,IF(AB2="",0,"?")))))))))*R2,2)</f>
+        <v/>
       </c>
       <c r="AM2">
-        <f t="shared" si="0"/>
-        <v>2.4</v>
+        <f>ROUND(IF(AC2="+",1,IF(AC2="+.",1,IF(AC2="+-",0.8,IF(AC2="+/2",0.5,IF(AC2="-+",0.1,IF(AC2="-.",0,IF(AC2="-",0,IF(AC2="0",0,IF(AC2="",0,"?")))))))))*S2,2)</f>
+        <v/>
       </c>
       <c r="AN2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AD2="+",1,IF(AD2="+.",1,IF(AD2="+-",0.8,IF(AD2="+/2",0.5,IF(AD2="-+",0.1,IF(AD2="-.",0,IF(AD2="-",0,IF(AD2="0",0,IF(AD2="",0,"?")))))))))*T2,2)</f>
+        <v/>
       </c>
       <c r="AO2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AE2="+",1,IF(AE2="+.",1,IF(AE2="+-",0.8,IF(AE2="+/2",0.5,IF(AE2="-+",0.1,IF(AE2="-.",0,IF(AE2="-",0,IF(AE2="0",0,IF(AE2="",0,"?")))))))))*U2,2)</f>
+        <v/>
       </c>
       <c r="AP2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AF2="+",1,IF(AF2="+.",1,IF(AF2="+-",0.8,IF(AF2="+/2",0.5,IF(AF2="-+",0.1,IF(AF2="-.",0,IF(AF2="-",0,IF(AF2="0",0,IF(AF2="",0,"?")))))))))*V2,2)</f>
+        <v/>
       </c>
       <c r="AQ2">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>ROUND(IF(AG2="+",1,IF(AG2="+.",1,IF(AG2="+-",0.8,IF(AG2="+/2",0.5,IF(AG2="-+",0.1,IF(AG2="-.",0,IF(AG2="-",0,IF(AG2="0",0,IF(AG2="",0,"?")))))))))*W2,2)</f>
+        <v/>
       </c>
       <c r="AR2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AH2="+",1,IF(AH2="+.",1,IF(AH2="+-",0.8,IF(AH2="+/2",0.5,IF(AH2="-+",0.1,IF(AH2="-.",0,IF(AH2="-",0,IF(AH2="0",0,IF(AH2="",0,"?")))))))))*X2,2)</f>
+        <v/>
       </c>
       <c r="AS2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AI2="+",1,IF(AI2="+.",1,IF(AI2="+-",0.8,IF(AI2="+/2",0.5,IF(AI2="-+",0.1,IF(AI2="-.",0,IF(AI2="-",0,IF(AI2="0",0,IF(AI2="",0,"?")))))))))*Y2,2)</f>
+        <v/>
       </c>
       <c r="AT2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AJ2="+",1,IF(AJ2="+.",1,IF(AJ2="+-",0.8,IF(AJ2="+/2",0.5,IF(AJ2="-+",0.1,IF(AJ2="-.",0,IF(AJ2="-",0,IF(AJ2="0",0,IF(AJ2="",0,"?")))))))))*Z2,2)</f>
+        <v/>
       </c>
       <c r="AU2" s="3">
         <f>SUM(AL2:AT2)</f>
-        <v>7.4</v>
+        <v/>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1106,13 +1109,13 @@
       <c r="E3" t="s">
         <v>63</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="n">
         <v>306</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="n">
         <v>234</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="n">
         <v>2002</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -1121,13 +1124,13 @@
       <c r="J3" t="s">
         <v>52</v>
       </c>
-      <c r="L3" t="str">
+      <c r="L3">
         <f>"Собеседования в 7-й математический класс 179-й школы"</f>
-        <v>Собеседования в 7-й математический класс 179-й школы</v>
-      </c>
-      <c r="M3" t="str">
+        <v/>
+      </c>
+      <c r="M3">
         <f>"|"</f>
-        <v>|</v>
+        <v/>
       </c>
       <c r="N3" t="s">
         <v>53</v>
@@ -1138,40 +1141,40 @@
       <c r="P3" t="s">
         <v>55</v>
       </c>
-      <c r="Q3" t="str">
+      <c r="Q3">
         <f>"|"</f>
-        <v>|</v>
-      </c>
-      <c r="R3">
-        <v>2</v>
-      </c>
-      <c r="S3">
-        <v>3</v>
-      </c>
-      <c r="T3">
-        <v>2</v>
-      </c>
-      <c r="U3">
-        <v>3</v>
-      </c>
-      <c r="V3">
-        <v>2</v>
-      </c>
-      <c r="W3">
-        <v>3</v>
-      </c>
-      <c r="X3">
-        <v>2</v>
-      </c>
-      <c r="Y3">
-        <v>3</v>
-      </c>
-      <c r="Z3">
+        <v/>
+      </c>
+      <c r="R3" t="n">
+        <v>2</v>
+      </c>
+      <c r="S3" t="n">
+        <v>3</v>
+      </c>
+      <c r="T3" t="n">
+        <v>2</v>
+      </c>
+      <c r="U3" t="n">
+        <v>3</v>
+      </c>
+      <c r="V3" t="n">
+        <v>2</v>
+      </c>
+      <c r="W3" t="n">
+        <v>3</v>
+      </c>
+      <c r="X3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z3" t="n">
         <v>2</v>
       </c>
       <c r="AA3" s="3">
         <f>SUM(R3:Z3)</f>
-        <v>22</v>
+        <v/>
       </c>
       <c r="AB3" s="1" t="s">
         <v>58</v>
@@ -1196,50 +1199,53 @@
       </c>
       <c r="AK3" s="3">
         <f>ROUND(IF(AB3="+",1,IF(AB3="+.",1,IF(AB3="+-",0.8,IF(AB3="+/2",0.5,IF(AB3="-+",0.1,IF(AB3="-.",0,IF(AB3="-",0,IF(AB3="0",0,IF(AB3="",0,"?")))))))))+IF(AC3="+",1,IF(AC3="+.",1,IF(AC3="+-",0.8,IF(AC3="+/2",0.5,IF(AC3="-+",0.1,IF(AC3="-.",0,IF(AC3="-",0,IF(AC3="0",0,IF(AC3="",0,"?")))))))))+IF(AD3="+",1,IF(AD3="+.",1,IF(AD3="+-",0.8,IF(AD3="+/2",0.5,IF(AD3="-+",0.1,IF(AD3="-.",0,IF(AD3="-",0,IF(AD3="0",0,IF(AD3="",0,"?")))))))))+IF(AE3="+",1,IF(AE3="+.",1,IF(AE3="+-",0.8,IF(AE3="+/2",0.5,IF(AE3="-+",0.1,IF(AE3="-.",0,IF(AE3="-",0,IF(AE3="0",0,IF(AE3="",0,"?")))))))))+IF(AF3="+",1,IF(AF3="+.",1,IF(AF3="+-",0.8,IF(AF3="+/2",0.5,IF(AF3="-+",0.1,IF(AF3="-.",0,IF(AF3="-",0,IF(AF3="0",0,IF(AF3="",0,"?")))))))))+IF(AG3="+",1,IF(AG3="+.",1,IF(AG3="+-",0.8,IF(AG3="+/2",0.5,IF(AG3="-+",0.1,IF(AG3="-.",0,IF(AG3="-",0,IF(AG3="0",0,IF(AG3="",0,"?")))))))))+IF(AH3="+",1,IF(AH3="+.",1,IF(AH3="+-",0.8,IF(AH3="+/2",0.5,IF(AH3="-+",0.1,IF(AH3="-.",0,IF(AH3="-",0,IF(AH3="0",0,IF(AH3="",0,"?")))))))))+IF(AI3="+",1,IF(AI3="+.",1,IF(AI3="+-",0.8,IF(AI3="+/2",0.5,IF(AI3="-+",0.1,IF(AI3="-.",0,IF(AI3="-",0,IF(AI3="0",0,IF(AI3="",0,"?")))))))))+IF(AJ3="+",1,IF(AJ3="+.",1,IF(AJ3="+-",0.8,IF(AJ3="+/2",0.5,IF(AJ3="-+",0.1,IF(AJ3="-.",0,IF(AJ3="-",0,IF(AJ3="0",0,IF(AJ3="",0,"?"))))))))),2)</f>
-        <v>3.5</v>
+        <v/>
       </c>
       <c r="AL3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AB3="+",1,IF(AB3="+.",1,IF(AB3="+-",0.8,IF(AB3="+/2",0.5,IF(AB3="-+",0.1,IF(AB3="-.",0,IF(AB3="-",0,IF(AB3="0",0,IF(AB3="",0,"?")))))))))*R3,2)</f>
+        <v/>
       </c>
       <c r="AM3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AC3="+",1,IF(AC3="+.",1,IF(AC3="+-",0.8,IF(AC3="+/2",0.5,IF(AC3="-+",0.1,IF(AC3="-.",0,IF(AC3="-",0,IF(AC3="0",0,IF(AC3="",0,"?")))))))))*S3,2)</f>
+        <v/>
       </c>
       <c r="AN3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>ROUND(IF(AD3="+",1,IF(AD3="+.",1,IF(AD3="+-",0.8,IF(AD3="+/2",0.5,IF(AD3="-+",0.1,IF(AD3="-.",0,IF(AD3="-",0,IF(AD3="0",0,IF(AD3="",0,"?")))))))))*T3,2)</f>
+        <v/>
       </c>
       <c r="AO3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>ROUND(IF(AE3="+",1,IF(AE3="+.",1,IF(AE3="+-",0.8,IF(AE3="+/2",0.5,IF(AE3="-+",0.1,IF(AE3="-.",0,IF(AE3="-",0,IF(AE3="0",0,IF(AE3="",0,"?")))))))))*U3,2)</f>
+        <v/>
       </c>
       <c r="AP3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>ROUND(IF(AF3="+",1,IF(AF3="+.",1,IF(AF3="+-",0.8,IF(AF3="+/2",0.5,IF(AF3="-+",0.1,IF(AF3="-.",0,IF(AF3="-",0,IF(AF3="0",0,IF(AF3="",0,"?")))))))))*V3,2)</f>
+        <v/>
       </c>
       <c r="AQ3">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
+        <f>ROUND(IF(AG3="+",1,IF(AG3="+.",1,IF(AG3="+-",0.8,IF(AG3="+/2",0.5,IF(AG3="-+",0.1,IF(AG3="-.",0,IF(AG3="-",0,IF(AG3="0",0,IF(AG3="",0,"?")))))))))*W3,2)</f>
+        <v/>
       </c>
       <c r="AR3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AH3="+",1,IF(AH3="+.",1,IF(AH3="+-",0.8,IF(AH3="+/2",0.5,IF(AH3="-+",0.1,IF(AH3="-.",0,IF(AH3="-",0,IF(AH3="0",0,IF(AH3="",0,"?")))))))))*X3,2)</f>
+        <v/>
       </c>
       <c r="AS3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AI3="+",1,IF(AI3="+.",1,IF(AI3="+-",0.8,IF(AI3="+/2",0.5,IF(AI3="-+",0.1,IF(AI3="-.",0,IF(AI3="-",0,IF(AI3="0",0,IF(AI3="",0,"?")))))))))*Y3,2)</f>
+        <v/>
       </c>
       <c r="AT3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AJ3="+",1,IF(AJ3="+.",1,IF(AJ3="+-",0.8,IF(AJ3="+/2",0.5,IF(AJ3="-+",0.1,IF(AJ3="-.",0,IF(AJ3="-",0,IF(AJ3="0",0,IF(AJ3="",0,"?")))))))))*Z3,2)</f>
+        <v/>
       </c>
       <c r="AU3" s="3">
         <f>SUM(AL3:AT3)</f>
-        <v>8.5</v>
+        <v/>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
       <c r="B4" t="s">
         <v>67</v>
       </c>
@@ -1252,13 +1258,13 @@
       <c r="E4" t="s">
         <v>70</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="n">
         <v>305</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="n">
         <v>123</v>
       </c>
-      <c r="H4">
+      <c r="H4" t="n">
         <v>2003</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -1267,13 +1273,13 @@
       <c r="J4" t="s">
         <v>52</v>
       </c>
-      <c r="L4" t="str">
+      <c r="L4">
         <f>"Собеседования в 7-й математический класс 179-й школы"</f>
-        <v>Собеседования в 7-й математический класс 179-й школы</v>
-      </c>
-      <c r="M4" t="str">
+        <v/>
+      </c>
+      <c r="M4">
         <f>"|"</f>
-        <v>|</v>
+        <v/>
       </c>
       <c r="N4" t="s">
         <v>53</v>
@@ -1284,40 +1290,40 @@
       <c r="P4" t="s">
         <v>55</v>
       </c>
-      <c r="Q4" t="str">
+      <c r="Q4">
         <f>"|"</f>
-        <v>|</v>
-      </c>
-      <c r="R4">
-        <v>2</v>
-      </c>
-      <c r="S4">
-        <v>3</v>
-      </c>
-      <c r="T4">
-        <v>2</v>
-      </c>
-      <c r="U4">
-        <v>3</v>
-      </c>
-      <c r="V4">
-        <v>2</v>
-      </c>
-      <c r="W4">
-        <v>3</v>
-      </c>
-      <c r="X4">
-        <v>2</v>
-      </c>
-      <c r="Y4">
-        <v>3</v>
-      </c>
-      <c r="Z4">
+        <v/>
+      </c>
+      <c r="R4" t="n">
+        <v>2</v>
+      </c>
+      <c r="S4" t="n">
+        <v>3</v>
+      </c>
+      <c r="T4" t="n">
+        <v>2</v>
+      </c>
+      <c r="U4" t="n">
+        <v>3</v>
+      </c>
+      <c r="V4" t="n">
+        <v>2</v>
+      </c>
+      <c r="W4" t="n">
+        <v>3</v>
+      </c>
+      <c r="X4" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z4" t="n">
         <v>2</v>
       </c>
       <c r="AA4" s="3">
         <f>SUM(R4:Z4)</f>
-        <v>22</v>
+        <v/>
       </c>
       <c r="AB4" s="1" t="s">
         <v>58</v>
@@ -1342,50 +1348,53 @@
       </c>
       <c r="AK4" s="3">
         <f>ROUND(IF(AB4="+",1,IF(AB4="+.",1,IF(AB4="+-",0.8,IF(AB4="+/2",0.5,IF(AB4="-+",0.1,IF(AB4="-.",0,IF(AB4="-",0,IF(AB4="0",0,IF(AB4="",0,"?")))))))))+IF(AC4="+",1,IF(AC4="+.",1,IF(AC4="+-",0.8,IF(AC4="+/2",0.5,IF(AC4="-+",0.1,IF(AC4="-.",0,IF(AC4="-",0,IF(AC4="0",0,IF(AC4="",0,"?")))))))))+IF(AD4="+",1,IF(AD4="+.",1,IF(AD4="+-",0.8,IF(AD4="+/2",0.5,IF(AD4="-+",0.1,IF(AD4="-.",0,IF(AD4="-",0,IF(AD4="0",0,IF(AD4="",0,"?")))))))))+IF(AE4="+",1,IF(AE4="+.",1,IF(AE4="+-",0.8,IF(AE4="+/2",0.5,IF(AE4="-+",0.1,IF(AE4="-.",0,IF(AE4="-",0,IF(AE4="0",0,IF(AE4="",0,"?")))))))))+IF(AF4="+",1,IF(AF4="+.",1,IF(AF4="+-",0.8,IF(AF4="+/2",0.5,IF(AF4="-+",0.1,IF(AF4="-.",0,IF(AF4="-",0,IF(AF4="0",0,IF(AF4="",0,"?")))))))))+IF(AG4="+",1,IF(AG4="+.",1,IF(AG4="+-",0.8,IF(AG4="+/2",0.5,IF(AG4="-+",0.1,IF(AG4="-.",0,IF(AG4="-",0,IF(AG4="0",0,IF(AG4="",0,"?")))))))))+IF(AH4="+",1,IF(AH4="+.",1,IF(AH4="+-",0.8,IF(AH4="+/2",0.5,IF(AH4="-+",0.1,IF(AH4="-.",0,IF(AH4="-",0,IF(AH4="0",0,IF(AH4="",0,"?")))))))))+IF(AI4="+",1,IF(AI4="+.",1,IF(AI4="+-",0.8,IF(AI4="+/2",0.5,IF(AI4="-+",0.1,IF(AI4="-.",0,IF(AI4="-",0,IF(AI4="0",0,IF(AI4="",0,"?")))))))))+IF(AJ4="+",1,IF(AJ4="+.",1,IF(AJ4="+-",0.8,IF(AJ4="+/2",0.5,IF(AJ4="-+",0.1,IF(AJ4="-.",0,IF(AJ4="-",0,IF(AJ4="0",0,IF(AJ4="",0,"?"))))))))),2)</f>
-        <v>5.0999999999999996</v>
+        <v/>
       </c>
       <c r="AL4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AB4="+",1,IF(AB4="+.",1,IF(AB4="+-",0.8,IF(AB4="+/2",0.5,IF(AB4="-+",0.1,IF(AB4="-.",0,IF(AB4="-",0,IF(AB4="0",0,IF(AB4="",0,"?")))))))))*R4,2)</f>
+        <v/>
       </c>
       <c r="AM4">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>ROUND(IF(AC4="+",1,IF(AC4="+.",1,IF(AC4="+-",0.8,IF(AC4="+/2",0.5,IF(AC4="-+",0.1,IF(AC4="-.",0,IF(AC4="-",0,IF(AC4="0",0,IF(AC4="",0,"?")))))))))*S4,2)</f>
+        <v/>
       </c>
       <c r="AN4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>ROUND(IF(AD4="+",1,IF(AD4="+.",1,IF(AD4="+-",0.8,IF(AD4="+/2",0.5,IF(AD4="-+",0.1,IF(AD4="-.",0,IF(AD4="-",0,IF(AD4="0",0,IF(AD4="",0,"?")))))))))*T4,2)</f>
+        <v/>
       </c>
       <c r="AO4">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>ROUND(IF(AE4="+",1,IF(AE4="+.",1,IF(AE4="+-",0.8,IF(AE4="+/2",0.5,IF(AE4="-+",0.1,IF(AE4="-.",0,IF(AE4="-",0,IF(AE4="0",0,IF(AE4="",0,"?")))))))))*U4,2)</f>
+        <v/>
       </c>
       <c r="AP4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>ROUND(IF(AF4="+",1,IF(AF4="+.",1,IF(AF4="+-",0.8,IF(AF4="+/2",0.5,IF(AF4="-+",0.1,IF(AF4="-.",0,IF(AF4="-",0,IF(AF4="0",0,IF(AF4="",0,"?")))))))))*V4,2)</f>
+        <v/>
       </c>
       <c r="AQ4">
-        <f t="shared" si="0"/>
-        <v>0.3</v>
+        <f>ROUND(IF(AG4="+",1,IF(AG4="+.",1,IF(AG4="+-",0.8,IF(AG4="+/2",0.5,IF(AG4="-+",0.1,IF(AG4="-.",0,IF(AG4="-",0,IF(AG4="0",0,IF(AG4="",0,"?")))))))))*W4,2)</f>
+        <v/>
       </c>
       <c r="AR4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>ROUND(IF(AH4="+",1,IF(AH4="+.",1,IF(AH4="+-",0.8,IF(AH4="+/2",0.5,IF(AH4="-+",0.1,IF(AH4="-.",0,IF(AH4="-",0,IF(AH4="0",0,IF(AH4="",0,"?")))))))))*X4,2)</f>
+        <v/>
       </c>
       <c r="AS4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AI4="+",1,IF(AI4="+.",1,IF(AI4="+-",0.8,IF(AI4="+/2",0.5,IF(AI4="-+",0.1,IF(AI4="-.",0,IF(AI4="-",0,IF(AI4="0",0,IF(AI4="",0,"?")))))))))*Y4,2)</f>
+        <v/>
       </c>
       <c r="AT4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AJ4="+",1,IF(AJ4="+.",1,IF(AJ4="+-",0.8,IF(AJ4="+/2",0.5,IF(AJ4="-+",0.1,IF(AJ4="-.",0,IF(AJ4="-",0,IF(AJ4="0",0,IF(AJ4="",0,"?")))))))))*Z4,2)</f>
+        <v/>
       </c>
       <c r="AU4" s="3">
         <f>SUM(AL4:AT4)</f>
-        <v>12.3</v>
+        <v/>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
       <c r="B5" t="s">
         <v>74</v>
       </c>
@@ -1398,13 +1407,13 @@
       <c r="E5" t="s">
         <v>76</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="n">
         <v>207</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="n">
         <v>432</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="n">
         <v>2004</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -1416,13 +1425,13 @@
       <c r="K5" t="s">
         <v>10</v>
       </c>
-      <c r="L5" t="str">
+      <c r="L5">
         <f>"Собеседования в 7-й математический класс 179-й школы"</f>
-        <v>Собеседования в 7-й математический класс 179-й школы</v>
-      </c>
-      <c r="M5" t="str">
+        <v/>
+      </c>
+      <c r="M5">
         <f>"|"</f>
-        <v>|</v>
+        <v/>
       </c>
       <c r="N5" t="s">
         <v>53</v>
@@ -1433,40 +1442,40 @@
       <c r="P5" t="s">
         <v>55</v>
       </c>
-      <c r="Q5" t="str">
+      <c r="Q5">
         <f>"|"</f>
-        <v>|</v>
-      </c>
-      <c r="R5">
-        <v>2</v>
-      </c>
-      <c r="S5">
-        <v>3</v>
-      </c>
-      <c r="T5">
-        <v>2</v>
-      </c>
-      <c r="U5">
-        <v>3</v>
-      </c>
-      <c r="V5">
-        <v>2</v>
-      </c>
-      <c r="W5">
-        <v>3</v>
-      </c>
-      <c r="X5">
-        <v>2</v>
-      </c>
-      <c r="Y5">
-        <v>3</v>
-      </c>
-      <c r="Z5">
+        <v/>
+      </c>
+      <c r="R5" t="n">
+        <v>2</v>
+      </c>
+      <c r="S5" t="n">
+        <v>3</v>
+      </c>
+      <c r="T5" t="n">
+        <v>2</v>
+      </c>
+      <c r="U5" t="n">
+        <v>3</v>
+      </c>
+      <c r="V5" t="n">
+        <v>2</v>
+      </c>
+      <c r="W5" t="n">
+        <v>3</v>
+      </c>
+      <c r="X5" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z5" t="n">
         <v>2</v>
       </c>
       <c r="AA5" s="3">
         <f>SUM(R5:Z5)</f>
-        <v>22</v>
+        <v/>
       </c>
       <c r="AB5" s="1" t="s">
         <v>56</v>
@@ -1491,47 +1500,47 @@
       </c>
       <c r="AK5" s="3">
         <f>ROUND(IF(AB5="+",1,IF(AB5="+.",1,IF(AB5="+-",0.8,IF(AB5="+/2",0.5,IF(AB5="-+",0.1,IF(AB5="-.",0,IF(AB5="-",0,IF(AB5="0",0,IF(AB5="",0,"?")))))))))+IF(AC5="+",1,IF(AC5="+.",1,IF(AC5="+-",0.8,IF(AC5="+/2",0.5,IF(AC5="-+",0.1,IF(AC5="-.",0,IF(AC5="-",0,IF(AC5="0",0,IF(AC5="",0,"?")))))))))+IF(AD5="+",1,IF(AD5="+.",1,IF(AD5="+-",0.8,IF(AD5="+/2",0.5,IF(AD5="-+",0.1,IF(AD5="-.",0,IF(AD5="-",0,IF(AD5="0",0,IF(AD5="",0,"?")))))))))+IF(AE5="+",1,IF(AE5="+.",1,IF(AE5="+-",0.8,IF(AE5="+/2",0.5,IF(AE5="-+",0.1,IF(AE5="-.",0,IF(AE5="-",0,IF(AE5="0",0,IF(AE5="",0,"?")))))))))+IF(AF5="+",1,IF(AF5="+.",1,IF(AF5="+-",0.8,IF(AF5="+/2",0.5,IF(AF5="-+",0.1,IF(AF5="-.",0,IF(AF5="-",0,IF(AF5="0",0,IF(AF5="",0,"?")))))))))+IF(AG5="+",1,IF(AG5="+.",1,IF(AG5="+-",0.8,IF(AG5="+/2",0.5,IF(AG5="-+",0.1,IF(AG5="-.",0,IF(AG5="-",0,IF(AG5="0",0,IF(AG5="",0,"?")))))))))+IF(AH5="+",1,IF(AH5="+.",1,IF(AH5="+-",0.8,IF(AH5="+/2",0.5,IF(AH5="-+",0.1,IF(AH5="-.",0,IF(AH5="-",0,IF(AH5="0",0,IF(AH5="",0,"?")))))))))+IF(AI5="+",1,IF(AI5="+.",1,IF(AI5="+-",0.8,IF(AI5="+/2",0.5,IF(AI5="-+",0.1,IF(AI5="-.",0,IF(AI5="-",0,IF(AI5="0",0,IF(AI5="",0,"?")))))))))+IF(AJ5="+",1,IF(AJ5="+.",1,IF(AJ5="+-",0.8,IF(AJ5="+/2",0.5,IF(AJ5="-+",0.1,IF(AJ5="-.",0,IF(AJ5="-",0,IF(AJ5="0",0,IF(AJ5="",0,"?"))))))))),2)</f>
-        <v>3</v>
+        <v/>
       </c>
       <c r="AL5">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>ROUND(IF(AB5="+",1,IF(AB5="+.",1,IF(AB5="+-",0.8,IF(AB5="+/2",0.5,IF(AB5="-+",0.1,IF(AB5="-.",0,IF(AB5="-",0,IF(AB5="0",0,IF(AB5="",0,"?")))))))))*R5,2)</f>
+        <v/>
       </c>
       <c r="AM5">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>ROUND(IF(AC5="+",1,IF(AC5="+.",1,IF(AC5="+-",0.8,IF(AC5="+/2",0.5,IF(AC5="-+",0.1,IF(AC5="-.",0,IF(AC5="-",0,IF(AC5="0",0,IF(AC5="",0,"?")))))))))*S5,2)</f>
+        <v/>
       </c>
       <c r="AN5">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>ROUND(IF(AD5="+",1,IF(AD5="+.",1,IF(AD5="+-",0.8,IF(AD5="+/2",0.5,IF(AD5="-+",0.1,IF(AD5="-.",0,IF(AD5="-",0,IF(AD5="0",0,IF(AD5="",0,"?")))))))))*T5,2)</f>
+        <v/>
       </c>
       <c r="AO5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AE5="+",1,IF(AE5="+.",1,IF(AE5="+-",0.8,IF(AE5="+/2",0.5,IF(AE5="-+",0.1,IF(AE5="-.",0,IF(AE5="-",0,IF(AE5="0",0,IF(AE5="",0,"?")))))))))*U5,2)</f>
+        <v/>
       </c>
       <c r="AP5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AF5="+",1,IF(AF5="+.",1,IF(AF5="+-",0.8,IF(AF5="+/2",0.5,IF(AF5="-+",0.1,IF(AF5="-.",0,IF(AF5="-",0,IF(AF5="0",0,IF(AF5="",0,"?")))))))))*V5,2)</f>
+        <v/>
       </c>
       <c r="AQ5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AG5="+",1,IF(AG5="+.",1,IF(AG5="+-",0.8,IF(AG5="+/2",0.5,IF(AG5="-+",0.1,IF(AG5="-.",0,IF(AG5="-",0,IF(AG5="0",0,IF(AG5="",0,"?")))))))))*W5,2)</f>
+        <v/>
       </c>
       <c r="AR5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AH5="+",1,IF(AH5="+.",1,IF(AH5="+-",0.8,IF(AH5="+/2",0.5,IF(AH5="-+",0.1,IF(AH5="-.",0,IF(AH5="-",0,IF(AH5="0",0,IF(AH5="",0,"?")))))))))*X5,2)</f>
+        <v/>
       </c>
       <c r="AS5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AI5="+",1,IF(AI5="+.",1,IF(AI5="+-",0.8,IF(AI5="+/2",0.5,IF(AI5="-+",0.1,IF(AI5="-.",0,IF(AI5="-",0,IF(AI5="0",0,IF(AI5="",0,"?")))))))))*Y5,2)</f>
+        <v/>
       </c>
       <c r="AT5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(IF(AJ5="+",1,IF(AJ5="+.",1,IF(AJ5="+-",0.8,IF(AJ5="+/2",0.5,IF(AJ5="-+",0.1,IF(AJ5="-.",0,IF(AJ5="-",0,IF(AJ5="0",0,IF(AJ5="",0,"?")))))))))*Z5,2)</f>
+        <v/>
       </c>
       <c r="AU5" s="3">
         <f>SUM(AL5:AT5)</f>
-        <v>7</v>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -1541,8 +1550,8 @@
     <hyperlink ref="I4" r:id="rId3"/>
     <hyperlink ref="I5" r:id="rId4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <tableParts count="1">
     <tablePart r:id="rId5"/>
   </tableParts>

</xml_diff>